<commit_message>
removed odometer and hours related columns from reports excel
</commit_message>
<xml_diff>
--- a/templates/export/trips.xlsx
+++ b/templates/export/trips.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDC21C-5B48-5745-8EFA-197BFCD822F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0929057-5BEC-B94D-8859-55DE30865E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="M7")</t>
+          <t>jx:area(lastCell="K7")</t>
         </r>
       </text>
     </comment>
@@ -49,7 +49,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="M7" multisheet="sheetNames")
+          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="K7" multisheet="sheetNames")
 </t>
         </r>
       </text>
@@ -64,7 +64,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="trip", lastCell="M7")</t>
+          <t>jx:each(items="device.objects", var="trip", lastCell="K7")</t>
         </r>
       </text>
     </comment>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Report type:</t>
   </si>
@@ -93,18 +93,12 @@
     <t>Start Address</t>
   </si>
   <si>
-    <t>Start Odometer</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
     <t>End Address</t>
   </si>
   <si>
-    <t>End Odometer</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -129,16 +123,10 @@
     <t>${util.hyperlink("".format("https://www.openstreetmap.org/?mlat=%1$f&amp;mlon=%2$f#map=16/%1$f/%2$f", trip.startLat, trip.startLon), trip.getStartAddress() == null ? "".format("%1$f°, %2$f°", trip.startLat, trip.startLon) : trip.startAddress)}</t>
   </si>
   <si>
-    <t xml:space="preserve">${distanceUnit.equals("mi") ? "".format("%.1f mi", trip.startOdometer * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", trip.startOdometer * 0.000539957) : "".format("%.1f km", trip.startOdometer * 0.001)} </t>
-  </si>
-  <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", trip.endTime, locale, timezone)}</t>
   </si>
   <si>
     <t>${util.hyperlink("".format("https://www.openstreetmap.org/?mlat=%1$f&amp;mlon=%2$f#map=16/%1$f/%2$f", trip.endLat, trip.endLon), trip.getEndAddress() == null ? "".format("%1$f°, %2$f°", trip.endLat, trip.endLon) : trip.endAddress)}</t>
-  </si>
-  <si>
-    <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", trip.endOdometer * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", trip.endOdometer * 0.000539957) : "".format("%.1f km", trip.endOdometer * 0.001)}</t>
   </si>
   <si>
     <t>${trip.duration/86400000.0}</t>
@@ -308,7 +296,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -829,17 +817,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M998"/>
+  <dimension ref="A1:K998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125"/>
     <col min="2" max="2" width="47.83203125"/>
-    <col min="3" max="3" width="17"/>
+    <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="20.83203125"/>
     <col min="5" max="5" width="50.33203125"/>
     <col min="6" max="6" width="19"/>
@@ -854,7 +842,7 @@
     <col min="29" max="1025" width="14.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -867,7 +855,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +872,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="3"/>
@@ -897,7 +885,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -914,7 +902,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="7"/>
       <c r="C5" s="3"/>
@@ -927,7 +915,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:13" s="9" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -959,54 +947,42 @@
         <v>13</v>
       </c>
       <c r="K6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="15" customFormat="1" ht="240" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="F7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="G7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="I7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="J7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update trip report excel row height
</commit_message>
<xml_diff>
--- a/templates/export/trips.xlsx
+++ b/templates/export/trips.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0929057-5BEC-B94D-8859-55DE30865E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9F5325-0E70-6248-A0B6-BBDFFB04E190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -950,7 +950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="15" customFormat="1" ht="240" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>

</xml_diff>